<commit_message>
pageviews ok tool in ga.py
</commit_message>
<xml_diff>
--- a/workhours.xlsx
+++ b/workhours.xlsx
@@ -74,10 +74,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -501,6 +502,22 @@
       <c r="C21" s="2">
         <v>0.4513888888888889</v>
       </c>
+      <c r="D21" s="2">
+        <v>0.54861111111111105</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="2">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0.76388888888888884</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C23" s="2">
+        <v>0.79166666666666663</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
barchart for datasets count is done in admin.py
</commit_message>
<xml_diff>
--- a/workhours.xlsx
+++ b/workhours.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>date</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>sum</t>
   </si>
 </sst>
 </file>
@@ -74,11 +77,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,15 +360,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -377,8 +381,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
         <v>42905</v>
       </c>
@@ -388,16 +395,34 @@
       <c r="D2" s="2">
         <v>0.70486111111111116</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="2">
+        <f>D2-C2</f>
+        <v>0.12152777777777779</v>
+      </c>
+      <c r="G2" s="4">
+        <f>SUM(E:E)</f>
+        <v>1.8124999999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C3" s="2">
         <v>0.87777777777777777</v>
       </c>
       <c r="D3" s="2">
         <v>0.95416666666666661</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3" s="2">
+        <f>D3-C3</f>
+        <v>7.638888888888884E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E4" s="2">
+        <f t="shared" ref="E4:E25" si="0">D4-C4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>42906</v>
       </c>
@@ -407,16 +432,30 @@
       <c r="D5" s="2">
         <v>0.52083333333333337</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5" s="2">
+        <f t="shared" si="0"/>
+        <v>9.3750000000000056E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C6" s="2">
         <v>0.54166666666666663</v>
       </c>
       <c r="D6" s="2">
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E7" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>42913</v>
       </c>
@@ -426,16 +465,30 @@
       <c r="D8" s="2">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666663</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C9" s="2">
         <v>0.83333333333333337</v>
       </c>
       <c r="D9" s="2">
         <v>0.91666666666666663</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333259E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>42914</v>
       </c>
@@ -445,16 +498,30 @@
       <c r="D11" s="2">
         <v>0.50694444444444442</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C12" s="2">
         <v>0.55555555555555558</v>
       </c>
       <c r="D12" s="2">
         <v>0.70138888888888884</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14583333333333326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>42915</v>
       </c>
@@ -464,8 +531,18 @@
       <c r="D14" s="2">
         <v>0.5625</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" s="2">
+        <f t="shared" si="0"/>
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>42922</v>
       </c>
@@ -475,16 +552,30 @@
       <c r="D16" s="2">
         <v>0.52777777777777779</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E16" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10416666666666669</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C17" s="2">
         <v>0.54861111111111105</v>
       </c>
       <c r="D17" s="2">
         <v>0.71180555555555547</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E17" s="2">
+        <f t="shared" si="0"/>
+        <v>0.16319444444444442</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E18" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
         <v>42923</v>
       </c>
@@ -494,8 +585,18 @@
       <c r="D19" s="2">
         <v>0.66666666666666663</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E19" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10416666666666663</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E20" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
         <v>42925</v>
       </c>
@@ -505,18 +606,54 @@
       <c r="D21" s="2">
         <v>0.54861111111111105</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E21" s="2">
+        <f t="shared" si="0"/>
+        <v>9.7222222222222154E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C22" s="2">
         <v>0.57638888888888895</v>
       </c>
       <c r="D22" s="3">
         <v>0.76388888888888884</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="E22" s="2">
+        <f t="shared" si="0"/>
+        <v>0.18749999999999989</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C23" s="2">
         <v>0.79166666666666663</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="E23" s="2">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E24" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="1">
+        <v>42926</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="E25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
world map cluster with infowindow on each marker
</commit_message>
<xml_diff>
--- a/workhours.xlsx
+++ b/workhours.xlsx
@@ -360,10 +360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -401,7 +401,7 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(E:E)</f>
-        <v>1.9062499999999996</v>
+        <v>2.114583333333333</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -418,7 +418,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E27" si="0">D4-C4</f>
+        <f t="shared" ref="E4:E28" si="0">D4-C4</f>
         <v>0</v>
       </c>
     </row>
@@ -680,6 +680,21 @@
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C28" s="2">
         <v>0.54166666666666663</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="E28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20833333333333337</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" s="1">
+        <v>42928</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.43055555555555558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
social button click tracker
</commit_message>
<xml_diff>
--- a/workhours.xlsx
+++ b/workhours.xlsx
@@ -363,13 +363,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -407,7 +410,7 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(E:E)</f>
-        <v>2.114583333333333</v>
+        <v>2.3090277777777772</v>
       </c>
       <c r="I2">
         <v>136</v>
@@ -427,7 +430,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E28" si="0">D4-C4</f>
+        <f t="shared" ref="E4:E31" si="0">D4-C4</f>
         <v>0</v>
       </c>
     </row>
@@ -698,6 +701,12 @@
         <v>0.20833333333333337</v>
       </c>
     </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E29" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <v>42928</v>
@@ -708,10 +717,26 @@
       <c r="D30" s="2">
         <v>0.52083333333333337</v>
       </c>
+      <c r="E30" s="2">
+        <f t="shared" si="0"/>
+        <v>9.027777777777779E-2</v>
+      </c>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C31" s="2">
         <v>0.58333333333333337</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="E31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.10416666666666663</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="1">
+        <v>42929</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tweet email actions send to GA OK
</commit_message>
<xml_diff>
--- a/workhours.xlsx
+++ b/workhours.xlsx
@@ -363,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -410,7 +410,7 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(E:E)</f>
-        <v>2.3090277777777772</v>
+        <v>2.5277777777777768</v>
       </c>
       <c r="I2">
         <v>136</v>
@@ -430,7 +430,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="E4" s="2">
-        <f t="shared" ref="E4:E31" si="0">D4-C4</f>
+        <f t="shared" ref="E4:E35" si="0">D4-C4</f>
         <v>0</v>
       </c>
     </row>
@@ -734,10 +734,41 @@
         <v>0.10416666666666663</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E32" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B33" s="1">
         <v>42929</v>
       </c>
+      <c r="C33" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D33" s="3">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="E33" s="2">
+        <f t="shared" si="0"/>
+        <v>7.2916666666666685E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C34" s="3">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="D34" s="3">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="E34" s="2">
+        <f t="shared" si="0"/>
+        <v>0.14583333333333326</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
doughnut chart for social clicks
</commit_message>
<xml_diff>
--- a/workhours.xlsx
+++ b/workhours.xlsx
@@ -366,7 +366,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -410,7 +410,7 @@
       </c>
       <c r="G2" s="4">
         <f>SUM(E:E)</f>
-        <v>2.5277777777777768</v>
+        <v>2.5895833333333322</v>
       </c>
       <c r="I2">
         <v>136</v>
@@ -768,7 +768,16 @@
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E35" s="2"/>
+      <c r="C35" s="3">
+        <v>0.9375</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E35" s="2">
+        <f t="shared" si="0"/>
+        <v>6.1805555555555558E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>